<commit_message>
Major petition data overhaul
</commit_message>
<xml_diff>
--- a/raw_data/jb_b2_0930.2019.xlsx
+++ b/raw_data/jb_b2_0930.2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Publications\Reports\Judicial Business\2019 Judicial Business\Writs of Certiorari\Appendix tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b874cf1d62adbd6e/Desktop/gov 50/final_project_test/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2875F7D0-76D1-4CC2-9E0A-DBFF0621615F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{D3E8BF10-4CDB-43B9-841D-8092B69FA6EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table B- 2" sheetId="1" r:id="rId1"/>
@@ -602,16 +602,16 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="6" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" customWidth="1"/>
+    <col min="8" max="8" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -622,7 +622,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -641,7 +641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -656,8 +656,8 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="2.5499999999999998" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="2.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -680,7 +680,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -703,7 +703,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -726,7 +726,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -749,7 +749,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -772,8 +772,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="2.5499999999999998" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="2.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -796,7 +796,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -842,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -865,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -911,7 +911,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -934,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -957,7 +957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -980,7 +980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>17</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>19</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>20</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>10</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>11</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>21</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>9</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>10</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>11</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>22</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>9</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>10</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>11</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>23</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>9</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>10</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>11</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>12</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>24</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>9</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>11</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>25</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>9</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>10</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>11</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="1" customFormat="1" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" s="1" customFormat="1" ht="11.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>12</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" ht="95.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7" s="1" customFormat="1" ht="95.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
         <v>27</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
     </row>
-    <row r="72" spans="1:7" s="1" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" spans="1:7" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:G1"/>

</xml_diff>